<commit_message>
updated activity log for 14th
</commit_message>
<xml_diff>
--- a/ActivityLog.xlsx
+++ b/ActivityLog.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madhu\Documents\restapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6B56216-4A32-4BF5-B52A-18ECA544B11F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C694EB93-8126-44ED-AB8B-C95888A95B6E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{76B3B90B-5595-4D4F-B0C0-6247B28E31D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Learning about REST APIs through youtube videos</t>
+  </si>
+  <si>
+    <t>Downloaded the requried software and configured eclipse to run this project.</t>
   </si>
 </sst>
 </file>
@@ -386,16 +389,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796626D9-8745-44C8-A17D-BA0CD2B91047}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.21875" customWidth="1"/>
+    <col min="2" max="2" width="62.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -414,6 +417,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>43538</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
All completed files added
</commit_message>
<xml_diff>
--- a/ActivityLog.xlsx
+++ b/ActivityLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madhu\Documents\restapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6B0A51-27F9-4D4F-B98A-538A39160AD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A1EB7B-978C-4D83-9FC4-D18D15C44A3E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{76B3B90B-5595-4D4F-B0C0-6247B28E31D7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Fixed few errors</t>
+  </si>
+  <si>
+    <t>Completed all three apis, fixed errors and recorded the demo video</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796626D9-8745-44C8-A17D-BA0CD2B91047}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,6 +483,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>43544</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>